<commit_message>
Latest update of files
</commit_message>
<xml_diff>
--- a/Code/Output/May_2020/RMA_Report_May_2020_2.xlsx
+++ b/Code/Output/May_2020/RMA_Report_May_2020_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\Output\May_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79EEC8E5-9018-40A3-B513-8D1AAA1E2C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DDDC5D-8970-4F5D-B311-CFDF0C9211A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="12375" yWindow="810" windowWidth="16980" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMA Reason Codes" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,11 @@
     <definedName name="_xlchart.v1.0" hidden="1">'RMA Reason Codes'!$H$2:$H$13</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'RMA Reason Codes'!$I$1</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'RMA Reason Codes'!$I$2:$I$13</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Driver and Engine RMAs'!$I$2:$I$20</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Driver and Engine RMAs'!$K$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Driver and Engine RMAs'!$K$2:$K$20</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Driver and Engine RMAs'!$I$24:$I$32</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Driver and Engine RMAs'!$K$24:$K$32</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Driver and Engine RMAs'!$I$24:$I$32</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Driver and Engine RMAs'!$K$24:$K$32</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Driver and Engine RMAs'!$I$2:$I$20</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Driver and Engine RMAs'!$K$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Driver and Engine RMAs'!$K$2:$K$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -852,10 +852,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -902,7 +902,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{CC090949-0A0F-416B-99E0-DA7BF34EEC19}" formatIdx="2">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>Qty</cx:v>
             </cx:txData>
           </cx:tx>
@@ -983,10 +983,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2836,7 +2836,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="1"/>
-              <a:ext cx="5953124" cy="3867149"/>
+              <a:ext cx="5953124" cy="3886199"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2913,7 +2913,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="3910012"/>
+              <a:off x="0" y="3929062"/>
               <a:ext cx="5953124" cy="2586038"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3616,7 +3616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B7600A-0572-4151-919D-5CF8CE548ABA}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="D23" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L35" sqref="L35:P45"/>
     </sheetView>
   </sheetViews>

</xml_diff>